<commit_message>
Made progress on visualization tonight
</commit_message>
<xml_diff>
--- a/loan_calculator.xlsx
+++ b/loan_calculator.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\volun\Documents\DA9\Capstone\capstone_da9_chase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6F07A1F-51C5-4B24-B2CF-AFC10A34ABB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB1729A9-C16E-4F14-A379-72899B1CA304}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{4F49E18B-FB22-4BA2-8D7F-0D5BA72B9504}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4F49E18B-FB22-4BA2-8D7F-0D5BA72B9504}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="44">
   <si>
     <t>Loan</t>
   </si>
@@ -156,6 +156,18 @@
   </si>
   <si>
     <t>x = 27.2</t>
+  </si>
+  <si>
+    <t>m = median salary</t>
+  </si>
+  <si>
+    <t>b = median salary * (age - 1)</t>
+  </si>
+  <si>
+    <t>31492.69 = 57539*22 + b</t>
+  </si>
+  <si>
+    <t>b = -1234365.31</t>
   </si>
 </sst>
 </file>
@@ -789,61 +801,61 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="25"/>
                 <c:pt idx="6" formatCode="0.00_);\(0.00\)">
-                  <c:v>28639.846644742334</c:v>
+                  <c:v>25856.080000000002</c:v>
                 </c:pt>
                 <c:pt idx="7" formatCode="0.00_);\(0.00\)">
-                  <c:v>70302.846644742327</c:v>
+                  <c:v>67519.08</c:v>
                 </c:pt>
                 <c:pt idx="8" formatCode="0.00_);\(0.00\)">
-                  <c:v>111965.84664474233</c:v>
+                  <c:v>109182.08</c:v>
                 </c:pt>
                 <c:pt idx="9" formatCode="0.00_);\(0.00\)">
-                  <c:v>153628.84664474233</c:v>
+                  <c:v>150845.08000000002</c:v>
                 </c:pt>
                 <c:pt idx="10" formatCode="0.00_);\(0.00\)">
-                  <c:v>195291.84664474233</c:v>
+                  <c:v>192508.08000000002</c:v>
                 </c:pt>
                 <c:pt idx="11" formatCode="0.00_);\(0.00\)">
-                  <c:v>236954.84664474233</c:v>
+                  <c:v>234171.08000000002</c:v>
                 </c:pt>
                 <c:pt idx="12" formatCode="0.00_);\(0.00\)">
-                  <c:v>278617.8466447423</c:v>
+                  <c:v>275834.08</c:v>
                 </c:pt>
                 <c:pt idx="13" formatCode="0.00_);\(0.00\)">
-                  <c:v>320280.8466447423</c:v>
+                  <c:v>317497.08</c:v>
                 </c:pt>
                 <c:pt idx="14" formatCode="0.00_);\(0.00\)">
-                  <c:v>361943.8466447423</c:v>
+                  <c:v>359160.08</c:v>
                 </c:pt>
                 <c:pt idx="15" formatCode="0.00_);\(0.00\)">
-                  <c:v>403606.8466447423</c:v>
+                  <c:v>400823.08</c:v>
                 </c:pt>
                 <c:pt idx="16" formatCode="0.00_);\(0.00\)">
-                  <c:v>445269.8466447423</c:v>
+                  <c:v>442486.08</c:v>
                 </c:pt>
                 <c:pt idx="17" formatCode="0.00_);\(0.00\)">
-                  <c:v>486932.8466447423</c:v>
+                  <c:v>484149.08</c:v>
                 </c:pt>
                 <c:pt idx="18" formatCode="0.00_);\(0.00\)">
-                  <c:v>528595.8466447423</c:v>
+                  <c:v>525812.08000000007</c:v>
                 </c:pt>
                 <c:pt idx="19" formatCode="0.00_);\(0.00\)">
-                  <c:v>570258.8466447423</c:v>
+                  <c:v>567475.08000000007</c:v>
                 </c:pt>
                 <c:pt idx="20" formatCode="0.00_);\(0.00\)">
-                  <c:v>611921.8466447423</c:v>
+                  <c:v>609138.08000000007</c:v>
                 </c:pt>
                 <c:pt idx="21" formatCode="0.00_);\(0.00\)">
-                  <c:v>653584.8466447423</c:v>
+                  <c:v>650801.08000000007</c:v>
                 </c:pt>
                 <c:pt idx="22" formatCode="0.00_);\(0.00\)">
-                  <c:v>695247.8466447423</c:v>
+                  <c:v>692464.08000000007</c:v>
                 </c:pt>
                 <c:pt idx="23" formatCode="0.00_);\(0.00\)">
-                  <c:v>736910.8466447423</c:v>
+                  <c:v>734127.08000000007</c:v>
                 </c:pt>
                 <c:pt idx="24" formatCode="0.00_);\(0.00\)">
-                  <c:v>778573.8466447423</c:v>
+                  <c:v>775790.08000000007</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -972,55 +984,55 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="25"/>
                 <c:pt idx="8" formatCode="0.00_);\(0.00\)">
-                  <c:v>31492.693289484665</c:v>
+                  <c:v>24198.750674038733</c:v>
                 </c:pt>
                 <c:pt idx="9" formatCode="0.00_);\(0.00\)">
-                  <c:v>89031.693289484669</c:v>
+                  <c:v>81737.750674038733</c:v>
                 </c:pt>
                 <c:pt idx="10" formatCode="0.00_);\(0.00\)">
-                  <c:v>146570.69328948465</c:v>
+                  <c:v>139276.75067403872</c:v>
                 </c:pt>
                 <c:pt idx="11" formatCode="0.00_);\(0.00\)">
-                  <c:v>204109.69328948465</c:v>
+                  <c:v>196815.75067403872</c:v>
                 </c:pt>
                 <c:pt idx="12" formatCode="0.00_);\(0.00\)">
-                  <c:v>261648.69328948465</c:v>
+                  <c:v>254354.75067403872</c:v>
                 </c:pt>
                 <c:pt idx="13" formatCode="0.00_);\(0.00\)">
-                  <c:v>319187.69328948465</c:v>
+                  <c:v>311893.75067403872</c:v>
                 </c:pt>
                 <c:pt idx="14" formatCode="0.00_);\(0.00\)">
-                  <c:v>376726.69328948465</c:v>
+                  <c:v>369432.75067403872</c:v>
                 </c:pt>
                 <c:pt idx="15" formatCode="0.00_);\(0.00\)">
-                  <c:v>434265.69328948465</c:v>
+                  <c:v>426971.75067403872</c:v>
                 </c:pt>
                 <c:pt idx="16" formatCode="0.00_);\(0.00\)">
-                  <c:v>491804.69328948465</c:v>
+                  <c:v>484510.75067403872</c:v>
                 </c:pt>
                 <c:pt idx="17" formatCode="0.00_);\(0.00\)">
-                  <c:v>549343.6932894846</c:v>
+                  <c:v>542049.75067403866</c:v>
                 </c:pt>
                 <c:pt idx="18" formatCode="0.00_);\(0.00\)">
-                  <c:v>606882.6932894846</c:v>
+                  <c:v>599588.75067403866</c:v>
                 </c:pt>
                 <c:pt idx="19" formatCode="0.00_);\(0.00\)">
-                  <c:v>664421.6932894846</c:v>
+                  <c:v>657127.75067403866</c:v>
                 </c:pt>
                 <c:pt idx="20" formatCode="0.00_);\(0.00\)">
-                  <c:v>721960.6932894846</c:v>
+                  <c:v>714666.75067403866</c:v>
                 </c:pt>
                 <c:pt idx="21" formatCode="0.00_);\(0.00\)">
-                  <c:v>779499.6932894846</c:v>
+                  <c:v>772205.75067403866</c:v>
                 </c:pt>
                 <c:pt idx="22" formatCode="0.00_);\(0.00\)">
-                  <c:v>837038.6932894846</c:v>
+                  <c:v>829744.75067403866</c:v>
                 </c:pt>
                 <c:pt idx="23" formatCode="0.00_);\(0.00\)">
-                  <c:v>894577.6932894846</c:v>
+                  <c:v>887283.75067403866</c:v>
                 </c:pt>
                 <c:pt idx="24" formatCode="0.00_);\(0.00\)">
-                  <c:v>952116.6932894846</c:v>
+                  <c:v>944822.75067403866</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1149,49 +1161,49 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="25"/>
                 <c:pt idx="10" formatCode="0.00_);\(0.00\)">
-                  <c:v>33767.539934226996</c:v>
+                  <c:v>22826.626011058099</c:v>
                 </c:pt>
                 <c:pt idx="11" formatCode="0.00_);\(0.00\)">
-                  <c:v>106604.539934227</c:v>
+                  <c:v>95663.626011058106</c:v>
                 </c:pt>
                 <c:pt idx="12" formatCode="0.00_);\(0.00\)">
-                  <c:v>179441.53993422701</c:v>
+                  <c:v>168500.62601105811</c:v>
                 </c:pt>
                 <c:pt idx="13" formatCode="0.00_);\(0.00\)">
-                  <c:v>252278.53993422701</c:v>
+                  <c:v>241337.62601105811</c:v>
                 </c:pt>
                 <c:pt idx="14" formatCode="0.00_);\(0.00\)">
-                  <c:v>325115.53993422701</c:v>
+                  <c:v>314174.62601105811</c:v>
                 </c:pt>
                 <c:pt idx="15" formatCode="0.00_);\(0.00\)">
-                  <c:v>397952.53993422701</c:v>
+                  <c:v>387011.62601105811</c:v>
                 </c:pt>
                 <c:pt idx="16" formatCode="0.00_);\(0.00\)">
-                  <c:v>470789.53993422701</c:v>
+                  <c:v>459848.62601105811</c:v>
                 </c:pt>
                 <c:pt idx="17" formatCode="0.00_);\(0.00\)">
-                  <c:v>543626.53993422701</c:v>
+                  <c:v>532685.62601105811</c:v>
                 </c:pt>
                 <c:pt idx="18" formatCode="0.00_);\(0.00\)">
-                  <c:v>616463.53993422701</c:v>
+                  <c:v>605522.62601105811</c:v>
                 </c:pt>
                 <c:pt idx="19" formatCode="0.00_);\(0.00\)">
-                  <c:v>689300.53993422701</c:v>
+                  <c:v>678359.62601105811</c:v>
                 </c:pt>
                 <c:pt idx="20" formatCode="0.00_);\(0.00\)">
-                  <c:v>762137.53993422701</c:v>
+                  <c:v>751196.62601105811</c:v>
                 </c:pt>
                 <c:pt idx="21" formatCode="0.00_);\(0.00\)">
-                  <c:v>834974.53993422701</c:v>
+                  <c:v>824033.62601105811</c:v>
                 </c:pt>
                 <c:pt idx="22" formatCode="0.00_);\(0.00\)">
-                  <c:v>907811.53993422701</c:v>
+                  <c:v>896870.62601105811</c:v>
                 </c:pt>
                 <c:pt idx="23" formatCode="0.00_);\(0.00\)">
-                  <c:v>980648.53993422701</c:v>
+                  <c:v>969707.62601105811</c:v>
                 </c:pt>
                 <c:pt idx="24" formatCode="0.00_);\(0.00\)">
-                  <c:v>1053485.539934227</c:v>
+                  <c:v>1042544.6260110581</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1949,61 +1961,61 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="25"/>
                 <c:pt idx="6" formatCode="0.00_);\(0.00\)">
-                  <c:v>34234.846644742334</c:v>
+                  <c:v>30587.875337019366</c:v>
                 </c:pt>
                 <c:pt idx="7" formatCode="0.00_);\(0.00\)">
-                  <c:v>81492.846644742327</c:v>
+                  <c:v>77845.875337019359</c:v>
                 </c:pt>
                 <c:pt idx="8" formatCode="0.00_);\(0.00\)">
-                  <c:v>128750.84664474233</c:v>
+                  <c:v>125103.87533701936</c:v>
                 </c:pt>
                 <c:pt idx="9" formatCode="0.00_);\(0.00\)">
-                  <c:v>176008.84664474233</c:v>
+                  <c:v>172361.87533701936</c:v>
                 </c:pt>
                 <c:pt idx="10" formatCode="0.00_);\(0.00\)">
-                  <c:v>223266.84664474233</c:v>
+                  <c:v>219619.87533701936</c:v>
                 </c:pt>
                 <c:pt idx="11" formatCode="0.00_);\(0.00\)">
-                  <c:v>270524.8466447423</c:v>
+                  <c:v>266877.87533701933</c:v>
                 </c:pt>
                 <c:pt idx="12" formatCode="0.00_);\(0.00\)">
-                  <c:v>317782.8466447423</c:v>
+                  <c:v>314135.87533701933</c:v>
                 </c:pt>
                 <c:pt idx="13" formatCode="0.00_);\(0.00\)">
-                  <c:v>365040.8466447423</c:v>
+                  <c:v>361393.87533701933</c:v>
                 </c:pt>
                 <c:pt idx="14" formatCode="0.00_);\(0.00\)">
-                  <c:v>412298.8466447423</c:v>
+                  <c:v>408651.87533701933</c:v>
                 </c:pt>
                 <c:pt idx="15" formatCode="0.00_);\(0.00\)">
-                  <c:v>459556.8466447423</c:v>
+                  <c:v>455909.87533701933</c:v>
                 </c:pt>
                 <c:pt idx="16" formatCode="0.00_);\(0.00\)">
-                  <c:v>506814.8466447423</c:v>
+                  <c:v>503167.87533701933</c:v>
                 </c:pt>
                 <c:pt idx="17" formatCode="0.00_);\(0.00\)">
-                  <c:v>554072.8466447423</c:v>
+                  <c:v>550425.87533701933</c:v>
                 </c:pt>
                 <c:pt idx="18" formatCode="0.00_);\(0.00\)">
-                  <c:v>601330.8466447423</c:v>
+                  <c:v>597683.87533701933</c:v>
                 </c:pt>
                 <c:pt idx="19" formatCode="0.00_);\(0.00\)">
-                  <c:v>648588.8466447423</c:v>
+                  <c:v>644941.87533701933</c:v>
                 </c:pt>
                 <c:pt idx="20" formatCode="0.00_);\(0.00\)">
-                  <c:v>695846.8466447423</c:v>
+                  <c:v>692199.87533701933</c:v>
                 </c:pt>
                 <c:pt idx="21" formatCode="0.00_);\(0.00\)">
-                  <c:v>743104.8466447423</c:v>
+                  <c:v>739457.87533701933</c:v>
                 </c:pt>
                 <c:pt idx="22" formatCode="0.00_);\(0.00\)">
-                  <c:v>790362.8466447423</c:v>
+                  <c:v>786715.87533701933</c:v>
                 </c:pt>
                 <c:pt idx="23" formatCode="0.00_);\(0.00\)">
-                  <c:v>837620.8466447423</c:v>
+                  <c:v>833973.87533701933</c:v>
                 </c:pt>
                 <c:pt idx="24" formatCode="0.00_);\(0.00\)">
-                  <c:v>884878.8466447423</c:v>
+                  <c:v>881231.87533701933</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2132,55 +2144,55 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="25"/>
                 <c:pt idx="8" formatCode="0.00_);\(0.00\)">
-                  <c:v>30783.693289484665</c:v>
+                  <c:v>23489.750674038733</c:v>
                 </c:pt>
                 <c:pt idx="9" formatCode="0.00_);\(0.00\)">
-                  <c:v>87613.693289484669</c:v>
+                  <c:v>80319.750674038733</c:v>
                 </c:pt>
                 <c:pt idx="10" formatCode="0.00_);\(0.00\)">
-                  <c:v>144443.69328948465</c:v>
+                  <c:v>137149.75067403872</c:v>
                 </c:pt>
                 <c:pt idx="11" formatCode="0.00_);\(0.00\)">
-                  <c:v>201273.69328948465</c:v>
+                  <c:v>193979.75067403872</c:v>
                 </c:pt>
                 <c:pt idx="12" formatCode="0.00_);\(0.00\)">
-                  <c:v>258103.69328948465</c:v>
+                  <c:v>250809.75067403872</c:v>
                 </c:pt>
                 <c:pt idx="13" formatCode="0.00_);\(0.00\)">
-                  <c:v>314933.69328948465</c:v>
+                  <c:v>307639.75067403872</c:v>
                 </c:pt>
                 <c:pt idx="14" formatCode="0.00_);\(0.00\)">
-                  <c:v>371763.69328948465</c:v>
+                  <c:v>364469.75067403872</c:v>
                 </c:pt>
                 <c:pt idx="15" formatCode="0.00_);\(0.00\)">
-                  <c:v>428593.69328948465</c:v>
+                  <c:v>421299.75067403872</c:v>
                 </c:pt>
                 <c:pt idx="16" formatCode="0.00_);\(0.00\)">
-                  <c:v>485423.69328948465</c:v>
+                  <c:v>478129.75067403872</c:v>
                 </c:pt>
                 <c:pt idx="17" formatCode="0.00_);\(0.00\)">
-                  <c:v>542253.6932894846</c:v>
+                  <c:v>534959.75067403866</c:v>
                 </c:pt>
                 <c:pt idx="18" formatCode="0.00_);\(0.00\)">
-                  <c:v>599083.6932894846</c:v>
+                  <c:v>591789.75067403866</c:v>
                 </c:pt>
                 <c:pt idx="19" formatCode="0.00_);\(0.00\)">
-                  <c:v>655913.6932894846</c:v>
+                  <c:v>648619.75067403866</c:v>
                 </c:pt>
                 <c:pt idx="20" formatCode="0.00_);\(0.00\)">
-                  <c:v>712743.6932894846</c:v>
+                  <c:v>705449.75067403866</c:v>
                 </c:pt>
                 <c:pt idx="21" formatCode="0.00_);\(0.00\)">
-                  <c:v>769573.6932894846</c:v>
+                  <c:v>762279.75067403866</c:v>
                 </c:pt>
                 <c:pt idx="22" formatCode="0.00_);\(0.00\)">
-                  <c:v>826403.6932894846</c:v>
+                  <c:v>819109.75067403866</c:v>
                 </c:pt>
                 <c:pt idx="23" formatCode="0.00_);\(0.00\)">
-                  <c:v>883233.6932894846</c:v>
+                  <c:v>875939.75067403866</c:v>
                 </c:pt>
                 <c:pt idx="24" formatCode="0.00_);\(0.00\)">
-                  <c:v>940063.6932894846</c:v>
+                  <c:v>932769.75067403866</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3503,16 +3515,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>449580</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>110490</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>7620</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>34290</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>175260</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>167640</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>777240</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>97155</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3875,8 +3887,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E7450C2-DD04-4E57-B93E-676584EB2405}">
   <dimension ref="A1:AI60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J33" sqref="J33"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3887,8 +3899,8 @@
     <col min="5" max="5" width="11.5546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.77734375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="23.6640625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="11.109375" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="13.21875" bestFit="1" customWidth="1"/>
@@ -4025,8 +4037,8 @@
       <c r="C4" s="5">
         <v>120</v>
       </c>
-      <c r="D4" s="4">
-        <v>20000</v>
+      <c r="D4">
+        <v>25600.75</v>
       </c>
       <c r="E4" s="2">
         <v>5.5E-2</v>
@@ -4037,15 +4049,15 @@
       </c>
       <c r="G4" s="4">
         <f>D4*F4</f>
-        <v>91.666666666666671</v>
+        <v>117.33677083333333</v>
       </c>
       <c r="H4" s="4">
         <f>D4*(F4/(1-(1+F4)^-C4))</f>
-        <v>217.05255592096111</v>
+        <v>277.83541104967725</v>
       </c>
       <c r="I4" s="4">
         <f>H4*C4</f>
-        <v>26046.306710515335</v>
+        <v>33340.249325961267</v>
       </c>
       <c r="L4">
         <v>14</v>
@@ -4064,6 +4076,34 @@
       </c>
     </row>
     <row r="5" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="B5">
+        <v>50000</v>
+      </c>
+      <c r="C5" s="5">
+        <v>120</v>
+      </c>
+      <c r="D5">
+        <v>10152.315789</v>
+      </c>
+      <c r="E5" s="2">
+        <v>5.5E-2</v>
+      </c>
+      <c r="F5" s="3">
+        <f>E5/12</f>
+        <v>4.5833333333333334E-3</v>
+      </c>
+      <c r="G5" s="4">
+        <f>D5*F5</f>
+        <v>46.531447366249999</v>
+      </c>
+      <c r="H5" s="4">
+        <f>D5*(F5/(1-(1+F5)^-C5))</f>
+        <v>110.17930452595895</v>
+      </c>
+      <c r="I5" s="4">
+        <f>H5*C5</f>
+        <v>13221.516543115074</v>
+      </c>
       <c r="L5">
         <v>15</v>
       </c>
@@ -4276,12 +4316,11 @@
         <v>41663</v>
       </c>
       <c r="X10" s="6">
-        <f>$I$4/2</f>
-        <v>13023.153355257667</v>
+        <v>15806.92</v>
       </c>
       <c r="Y10" s="7">
         <f>W10-X10</f>
-        <v>28639.846644742334</v>
+        <v>25856.080000000002</v>
       </c>
       <c r="AA10">
         <v>20</v>
@@ -4332,12 +4371,12 @@
         <v>41663</v>
       </c>
       <c r="X11" s="6">
-        <f>X10-(($H$4*12)/2)</f>
-        <v>11720.8380197319</v>
+        <f>X10-($X$10*0.1)</f>
+        <v>14226.227999999999</v>
       </c>
       <c r="Y11" s="7">
         <f>W11+Y10</f>
-        <v>70302.846644742327</v>
+        <v>67519.08</v>
       </c>
       <c r="AA11">
         <v>21</v>
@@ -4392,12 +4431,12 @@
         <v>41663</v>
       </c>
       <c r="X12" s="6">
-        <f t="shared" ref="X12:X20" si="2">X11-(($H$4*12)/2)</f>
-        <v>10418.522684206133</v>
+        <f t="shared" ref="X12:X20" si="2">X11-($X$10*0.1)</f>
+        <v>12645.536</v>
       </c>
       <c r="Y12" s="7">
         <f>W12+Y11</f>
-        <v>111965.84664474233</v>
+        <v>109182.08</v>
       </c>
       <c r="AA12">
         <v>22</v>
@@ -4407,11 +4446,11 @@
       </c>
       <c r="AC12" s="6">
         <f>$I$4</f>
-        <v>26046.306710515335</v>
+        <v>33340.249325961267</v>
       </c>
       <c r="AD12" s="7">
         <f>AB12-AC12</f>
-        <v>31492.693289484665</v>
+        <v>24198.750674038733</v>
       </c>
       <c r="AF12">
         <v>22</v>
@@ -4454,11 +4493,11 @@
       </c>
       <c r="X13" s="6">
         <f t="shared" si="2"/>
-        <v>9116.2073486803656</v>
+        <v>11064.844000000001</v>
       </c>
       <c r="Y13" s="7">
         <f t="shared" ref="Y13:Y28" si="3">W13+Y12</f>
-        <v>153628.84664474233</v>
+        <v>150845.08000000002</v>
       </c>
       <c r="AA13">
         <v>23</v>
@@ -4468,11 +4507,11 @@
       </c>
       <c r="AC13" s="6">
         <f>AC12-($H$4*12)</f>
-        <v>23441.6760394638</v>
+        <v>30006.224393365141</v>
       </c>
       <c r="AD13" s="7">
         <f>AB13+AD12</f>
-        <v>89031.693289484669</v>
+        <v>81737.750674038733</v>
       </c>
       <c r="AF13">
         <v>23</v>
@@ -4518,11 +4557,11 @@
       </c>
       <c r="X14" s="6">
         <f t="shared" si="2"/>
-        <v>7813.8920131545992</v>
+        <v>9484.1520000000019</v>
       </c>
       <c r="Y14" s="7">
         <f t="shared" si="3"/>
-        <v>195291.84664474233</v>
+        <v>192508.08000000002</v>
       </c>
       <c r="AA14">
         <v>24</v>
@@ -4532,11 +4571,11 @@
       </c>
       <c r="AC14" s="6">
         <f t="shared" ref="AC14:AC22" si="4">AC13-($H$4*12)</f>
-        <v>20837.045368412266</v>
+        <v>26672.199460769014</v>
       </c>
       <c r="AD14" s="7">
         <f>AB14+AD13</f>
-        <v>146570.69328948465</v>
+        <v>139276.75067403872</v>
       </c>
       <c r="AF14">
         <v>24</v>
@@ -4546,11 +4585,11 @@
       </c>
       <c r="AH14" s="6">
         <f>I4*1.5</f>
-        <v>39069.460065773004</v>
+        <v>50010.373988941901</v>
       </c>
       <c r="AI14" s="7">
         <f>AG14-AH14</f>
-        <v>33767.539934226996</v>
+        <v>22826.626011058099</v>
       </c>
     </row>
     <row r="15" spans="1:35" x14ac:dyDescent="0.3">
@@ -4583,11 +4622,11 @@
       </c>
       <c r="X15" s="6">
         <f t="shared" si="2"/>
-        <v>6511.5766776288328</v>
+        <v>7903.4600000000019</v>
       </c>
       <c r="Y15" s="7">
         <f t="shared" si="3"/>
-        <v>236954.84664474233</v>
+        <v>234171.08000000002</v>
       </c>
       <c r="AA15">
         <v>25</v>
@@ -4597,11 +4636,11 @@
       </c>
       <c r="AC15" s="6">
         <f t="shared" si="4"/>
-        <v>18232.414697360731</v>
+        <v>23338.174528172887</v>
       </c>
       <c r="AD15" s="7">
         <f t="shared" ref="AD15:AD28" si="5">AB15+AD14</f>
-        <v>204109.69328948465</v>
+        <v>196815.75067403872</v>
       </c>
       <c r="AF15">
         <v>25</v>
@@ -4611,11 +4650,11 @@
       </c>
       <c r="AH15" s="6">
         <f>AH14-($H$4*12*1.5)</f>
-        <v>35162.514059195702</v>
+        <v>45009.336590047707</v>
       </c>
       <c r="AI15" s="7">
         <f t="shared" ref="AI15:AI28" si="6">AG15+AI14</f>
-        <v>106604.539934227</v>
+        <v>95663.626011058106</v>
       </c>
     </row>
     <row r="16" spans="1:35" x14ac:dyDescent="0.3">
@@ -4651,11 +4690,11 @@
       </c>
       <c r="X16" s="6">
         <f t="shared" si="2"/>
-        <v>5209.2613421030665</v>
+        <v>6322.7680000000018</v>
       </c>
       <c r="Y16" s="7">
         <f t="shared" si="3"/>
-        <v>278617.8466447423</v>
+        <v>275834.08</v>
       </c>
       <c r="AA16">
         <v>26</v>
@@ -4665,11 +4704,11 @@
       </c>
       <c r="AC16" s="6">
         <f t="shared" si="4"/>
-        <v>15627.784026309198</v>
+        <v>20004.14959557676</v>
       </c>
       <c r="AD16" s="7">
         <f t="shared" si="5"/>
-        <v>261648.69328948465</v>
+        <v>254354.75067403872</v>
       </c>
       <c r="AF16">
         <v>26</v>
@@ -4679,14 +4718,14 @@
       </c>
       <c r="AH16" s="6">
         <f t="shared" ref="AH16:AH24" si="7">AH15-($H$4*12*1.5)</f>
-        <v>31255.568052618401</v>
+        <v>40008.299191153521</v>
       </c>
       <c r="AI16" s="7">
         <f t="shared" si="6"/>
-        <v>179441.53993422701</v>
+        <v>168500.62601105811</v>
       </c>
     </row>
-    <row r="17" spans="9:35" x14ac:dyDescent="0.3">
+    <row r="17" spans="8:35" x14ac:dyDescent="0.3">
       <c r="L17">
         <v>27</v>
       </c>
@@ -4716,11 +4755,11 @@
       </c>
       <c r="X17" s="6">
         <f t="shared" si="2"/>
-        <v>3906.9460065773001</v>
+        <v>4742.0760000000018</v>
       </c>
       <c r="Y17" s="7">
         <f t="shared" si="3"/>
-        <v>320280.8466447423</v>
+        <v>317497.08</v>
       </c>
       <c r="AA17">
         <v>27</v>
@@ -4730,11 +4769,11 @@
       </c>
       <c r="AC17" s="6">
         <f t="shared" si="4"/>
-        <v>13023.153355257666</v>
+        <v>16670.124662980634</v>
       </c>
       <c r="AD17" s="7">
         <f t="shared" si="5"/>
-        <v>319187.69328948465</v>
+        <v>311893.75067403872</v>
       </c>
       <c r="AF17">
         <v>27</v>
@@ -4744,14 +4783,14 @@
       </c>
       <c r="AH17" s="6">
         <f t="shared" si="7"/>
-        <v>27348.622046041099</v>
+        <v>35007.261792259334</v>
       </c>
       <c r="AI17" s="7">
         <f t="shared" si="6"/>
-        <v>252278.53993422701</v>
+        <v>241337.62601105811</v>
       </c>
     </row>
-    <row r="18" spans="9:35" x14ac:dyDescent="0.3">
+    <row r="18" spans="8:35" x14ac:dyDescent="0.3">
       <c r="L18">
         <v>28</v>
       </c>
@@ -4781,11 +4820,11 @@
       </c>
       <c r="X18" s="6">
         <f t="shared" si="2"/>
-        <v>2604.6306710515337</v>
+        <v>3161.3840000000018</v>
       </c>
       <c r="Y18" s="7">
         <f t="shared" si="3"/>
-        <v>361943.8466447423</v>
+        <v>359160.08</v>
       </c>
       <c r="AA18">
         <v>28</v>
@@ -4795,11 +4834,11 @@
       </c>
       <c r="AC18" s="6">
         <f t="shared" si="4"/>
-        <v>10418.522684206133</v>
+        <v>13336.099730384507</v>
       </c>
       <c r="AD18" s="7">
         <f t="shared" si="5"/>
-        <v>376726.69328948465</v>
+        <v>369432.75067403872</v>
       </c>
       <c r="AF18">
         <v>28</v>
@@ -4809,14 +4848,14 @@
       </c>
       <c r="AH18" s="6">
         <f t="shared" si="7"/>
-        <v>23441.676039463797</v>
+        <v>30006.224393365144</v>
       </c>
       <c r="AI18" s="7">
         <f t="shared" si="6"/>
-        <v>325115.53993422701</v>
+        <v>314174.62601105811</v>
       </c>
     </row>
-    <row r="19" spans="9:35" x14ac:dyDescent="0.3">
+    <row r="19" spans="8:35" x14ac:dyDescent="0.3">
       <c r="J19" s="8" t="s">
         <v>25</v>
       </c>
@@ -4852,11 +4891,11 @@
       </c>
       <c r="X19" s="6">
         <f t="shared" si="2"/>
-        <v>1302.3153355257671</v>
+        <v>1580.6920000000018</v>
       </c>
       <c r="Y19" s="7">
         <f t="shared" si="3"/>
-        <v>403606.8466447423</v>
+        <v>400823.08</v>
       </c>
       <c r="AA19">
         <v>29</v>
@@ -4866,11 +4905,11 @@
       </c>
       <c r="AC19" s="6">
         <f t="shared" si="4"/>
-        <v>7813.8920131546001</v>
+        <v>10002.07479778838</v>
       </c>
       <c r="AD19" s="7">
         <f t="shared" si="5"/>
-        <v>434265.69328948465</v>
+        <v>426971.75067403872</v>
       </c>
       <c r="AF19">
         <v>29</v>
@@ -4880,14 +4919,14 @@
       </c>
       <c r="AH19" s="6">
         <f t="shared" si="7"/>
-        <v>19534.730032886495</v>
+        <v>25005.186994470954</v>
       </c>
       <c r="AI19" s="7">
         <f t="shared" si="6"/>
-        <v>397952.53993422701</v>
+        <v>387011.62601105811</v>
       </c>
     </row>
-    <row r="20" spans="9:35" x14ac:dyDescent="0.3">
+    <row r="20" spans="8:35" x14ac:dyDescent="0.3">
       <c r="J20" t="s">
         <v>27</v>
       </c>
@@ -4923,11 +4962,11 @@
       </c>
       <c r="X20" s="6">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1.8189894035458565E-12</v>
       </c>
       <c r="Y20" s="7">
         <f t="shared" si="3"/>
-        <v>445269.8466447423</v>
+        <v>442486.08</v>
       </c>
       <c r="AA20">
         <v>30</v>
@@ -4937,11 +4976,11 @@
       </c>
       <c r="AC20" s="6">
         <f t="shared" si="4"/>
-        <v>5209.2613421030674</v>
+        <v>6668.0498651922535</v>
       </c>
       <c r="AD20" s="7">
         <f t="shared" si="5"/>
-        <v>491804.69328948465</v>
+        <v>484510.75067403872</v>
       </c>
       <c r="AF20">
         <v>30</v>
@@ -4951,14 +4990,14 @@
       </c>
       <c r="AH20" s="6">
         <f t="shared" si="7"/>
-        <v>15627.784026309195</v>
+        <v>20004.149595576764</v>
       </c>
       <c r="AI20" s="7">
         <f t="shared" si="6"/>
-        <v>470789.53993422701</v>
+        <v>459848.62601105811</v>
       </c>
     </row>
-    <row r="21" spans="9:35" x14ac:dyDescent="0.3">
+    <row r="21" spans="8:35" x14ac:dyDescent="0.3">
       <c r="J21" s="8" t="s">
         <v>29</v>
       </c>
@@ -4992,7 +5031,7 @@
       <c r="X21" s="6"/>
       <c r="Y21" s="7">
         <f t="shared" si="3"/>
-        <v>486932.8466447423</v>
+        <v>484149.08</v>
       </c>
       <c r="AA21">
         <v>31</v>
@@ -5002,11 +5041,11 @@
       </c>
       <c r="AC21" s="6">
         <f t="shared" si="4"/>
-        <v>2604.6306710515341</v>
+        <v>3334.0249325961267</v>
       </c>
       <c r="AD21" s="7">
         <f t="shared" si="5"/>
-        <v>549343.6932894846</v>
+        <v>542049.75067403866</v>
       </c>
       <c r="AF21">
         <v>31</v>
@@ -5016,14 +5055,14 @@
       </c>
       <c r="AH21" s="6">
         <f t="shared" si="7"/>
-        <v>11720.838019731895</v>
+        <v>15003.112196682574</v>
       </c>
       <c r="AI21" s="7">
         <f t="shared" si="6"/>
-        <v>543626.53993422701</v>
+        <v>532685.62601105811</v>
       </c>
     </row>
-    <row r="22" spans="9:35" x14ac:dyDescent="0.3">
+    <row r="22" spans="8:35" x14ac:dyDescent="0.3">
       <c r="J22" s="8" t="s">
         <v>30</v>
       </c>
@@ -5057,7 +5096,7 @@
       <c r="X22" s="6"/>
       <c r="Y22" s="7">
         <f t="shared" si="3"/>
-        <v>528595.8466447423</v>
+        <v>525812.08000000007</v>
       </c>
       <c r="AA22">
         <v>32</v>
@@ -5071,7 +5110,7 @@
       </c>
       <c r="AD22" s="7">
         <f t="shared" si="5"/>
-        <v>606882.6932894846</v>
+        <v>599588.75067403866</v>
       </c>
       <c r="AF22">
         <v>32</v>
@@ -5081,14 +5120,14 @@
       </c>
       <c r="AH22" s="6">
         <f t="shared" si="7"/>
-        <v>7813.8920131545947</v>
+        <v>10002.074797788384</v>
       </c>
       <c r="AI22" s="7">
         <f t="shared" si="6"/>
-        <v>616463.53993422701</v>
+        <v>605522.62601105811</v>
       </c>
     </row>
-    <row r="23" spans="9:35" x14ac:dyDescent="0.3">
+    <row r="23" spans="8:35" x14ac:dyDescent="0.3">
       <c r="J23" s="8" t="s">
         <v>31</v>
       </c>
@@ -5122,7 +5161,7 @@
       <c r="X23" s="6"/>
       <c r="Y23" s="7">
         <f t="shared" si="3"/>
-        <v>570258.8466447423</v>
+        <v>567475.08000000007</v>
       </c>
       <c r="AA23">
         <v>33</v>
@@ -5133,7 +5172,7 @@
       <c r="AC23" s="6"/>
       <c r="AD23" s="7">
         <f t="shared" si="5"/>
-        <v>664421.6932894846</v>
+        <v>657127.75067403866</v>
       </c>
       <c r="AF23">
         <v>33</v>
@@ -5143,14 +5182,14 @@
       </c>
       <c r="AH23" s="6">
         <f t="shared" si="7"/>
-        <v>3906.9460065772946</v>
+        <v>5001.0373988941938</v>
       </c>
       <c r="AI23" s="7">
         <f t="shared" si="6"/>
-        <v>689300.53993422701</v>
+        <v>678359.62601105811</v>
       </c>
     </row>
-    <row r="24" spans="9:35" x14ac:dyDescent="0.3">
+    <row r="24" spans="8:35" x14ac:dyDescent="0.3">
       <c r="J24" s="8" t="s">
         <v>32</v>
       </c>
@@ -5184,7 +5223,7 @@
       <c r="X24" s="6"/>
       <c r="Y24" s="7">
         <f t="shared" si="3"/>
-        <v>611921.8466447423</v>
+        <v>609138.08000000007</v>
       </c>
       <c r="AA24">
         <v>34</v>
@@ -5195,7 +5234,7 @@
       <c r="AC24" s="6"/>
       <c r="AD24" s="7">
         <f t="shared" si="5"/>
-        <v>721960.6932894846</v>
+        <v>714666.75067403866</v>
       </c>
       <c r="AF24">
         <v>34</v>
@@ -5205,14 +5244,17 @@
       </c>
       <c r="AH24" s="6">
         <f t="shared" si="7"/>
-        <v>-5.4569682106375694E-12</v>
+        <v>0</v>
       </c>
       <c r="AI24" s="7">
         <f t="shared" si="6"/>
-        <v>762137.53993422701</v>
+        <v>751196.62601105811</v>
       </c>
     </row>
-    <row r="25" spans="9:35" x14ac:dyDescent="0.3">
+    <row r="25" spans="8:35" x14ac:dyDescent="0.3">
+      <c r="H25" t="s">
+        <v>40</v>
+      </c>
       <c r="I25">
         <f>60366-30183</f>
         <v>30183</v>
@@ -5248,7 +5290,7 @@
       </c>
       <c r="Y25" s="7">
         <f t="shared" si="3"/>
-        <v>653584.8466447423</v>
+        <v>650801.08000000007</v>
       </c>
       <c r="AA25">
         <v>35</v>
@@ -5258,7 +5300,7 @@
       </c>
       <c r="AD25" s="7">
         <f t="shared" si="5"/>
-        <v>779499.6932894846</v>
+        <v>772205.75067403866</v>
       </c>
       <c r="AF25">
         <v>35</v>
@@ -5268,10 +5310,13 @@
       </c>
       <c r="AI25" s="7">
         <f t="shared" si="6"/>
-        <v>834974.53993422701</v>
+        <v>824033.62601105811</v>
       </c>
     </row>
-    <row r="26" spans="9:35" x14ac:dyDescent="0.3">
+    <row r="26" spans="8:35" x14ac:dyDescent="0.3">
+      <c r="H26" t="s">
+        <v>41</v>
+      </c>
       <c r="I26">
         <f>I25*16</f>
         <v>482928</v>
@@ -5307,7 +5352,7 @@
       </c>
       <c r="Y26" s="7">
         <f t="shared" si="3"/>
-        <v>695247.8466447423</v>
+        <v>692464.08000000007</v>
       </c>
       <c r="AA26">
         <v>36</v>
@@ -5317,7 +5362,7 @@
       </c>
       <c r="AD26" s="7">
         <f t="shared" si="5"/>
-        <v>837038.6932894846</v>
+        <v>829744.75067403866</v>
       </c>
       <c r="AF26">
         <v>36</v>
@@ -5327,10 +5372,14 @@
       </c>
       <c r="AI26" s="7">
         <f t="shared" si="6"/>
-        <v>907811.53993422701</v>
+        <v>896870.62601105811</v>
       </c>
     </row>
-    <row r="27" spans="9:35" x14ac:dyDescent="0.3">
+    <row r="27" spans="8:35" x14ac:dyDescent="0.3">
+      <c r="H27">
+        <f>I25*15</f>
+        <v>452745</v>
+      </c>
       <c r="I27">
         <f>I25-I26</f>
         <v>-452745</v>
@@ -5366,7 +5415,7 @@
       </c>
       <c r="Y27" s="7">
         <f t="shared" si="3"/>
-        <v>736910.8466447423</v>
+        <v>734127.08000000007</v>
       </c>
       <c r="AA27">
         <v>37</v>
@@ -5376,7 +5425,7 @@
       </c>
       <c r="AD27" s="7">
         <f t="shared" si="5"/>
-        <v>894577.6932894846</v>
+        <v>887283.75067403866</v>
       </c>
       <c r="AF27">
         <v>37</v>
@@ -5386,10 +5435,10 @@
       </c>
       <c r="AI27" s="7">
         <f t="shared" si="6"/>
-        <v>980648.53993422701</v>
+        <v>969707.62601105811</v>
       </c>
     </row>
-    <row r="28" spans="9:35" x14ac:dyDescent="0.3">
+    <row r="28" spans="8:35" x14ac:dyDescent="0.3">
       <c r="L28">
         <v>38</v>
       </c>
@@ -5418,7 +5467,7 @@
       </c>
       <c r="Y28" s="7">
         <f t="shared" si="3"/>
-        <v>778573.8466447423</v>
+        <v>775790.08000000007</v>
       </c>
       <c r="AA28">
         <v>38</v>
@@ -5428,7 +5477,11 @@
       </c>
       <c r="AD28" s="7">
         <f t="shared" si="5"/>
-        <v>952116.6932894846</v>
+        <v>944822.75067403866</v>
+      </c>
+      <c r="AE28">
+        <f>(((AA28-AA12)*AB28)+AD12)</f>
+        <v>944822.75067403878</v>
       </c>
       <c r="AF28">
         <v>38</v>
@@ -5438,21 +5491,71 @@
       </c>
       <c r="AI28" s="7">
         <f t="shared" si="6"/>
-        <v>1053485.539934227</v>
+        <v>1042544.6260110581</v>
       </c>
     </row>
-    <row r="29" spans="9:35" x14ac:dyDescent="0.3">
+    <row r="29" spans="8:35" x14ac:dyDescent="0.3">
       <c r="J29" t="s">
         <v>36</v>
       </c>
+      <c r="L29">
+        <v>39</v>
+      </c>
+      <c r="M29">
+        <v>30183</v>
+      </c>
+      <c r="O29" s="7">
+        <f t="shared" ref="O29" si="8">O28+M29</f>
+        <v>724392</v>
+      </c>
+      <c r="Q29">
+        <v>39</v>
+      </c>
+      <c r="R29">
+        <v>36093</v>
+      </c>
+      <c r="T29" s="7">
+        <f t="shared" ref="T29" si="9">T28+R29</f>
+        <v>794046</v>
+      </c>
+      <c r="V29">
+        <v>39</v>
+      </c>
+      <c r="W29">
+        <v>41663</v>
+      </c>
+      <c r="Y29" s="7">
+        <f t="shared" ref="Y29" si="10">W29+Y28</f>
+        <v>817453.08000000007</v>
+      </c>
+      <c r="AA29">
+        <v>39</v>
+      </c>
+      <c r="AB29">
+        <v>57539</v>
+      </c>
+      <c r="AD29" s="7">
+        <f t="shared" ref="AD29" si="11">AB29+AD28</f>
+        <v>1002361.7506740387</v>
+      </c>
+      <c r="AF29">
+        <v>39</v>
+      </c>
+      <c r="AG29">
+        <v>72837</v>
+      </c>
+      <c r="AI29" s="7">
+        <f t="shared" ref="AI29" si="12">AG29+AI28</f>
+        <v>1115381.6260110582</v>
+      </c>
     </row>
-    <row r="30" spans="9:35" x14ac:dyDescent="0.3">
+    <row r="30" spans="8:35" x14ac:dyDescent="0.3">
       <c r="I30">
         <f>36093*17</f>
         <v>613581</v>
       </c>
     </row>
-    <row r="31" spans="9:35" x14ac:dyDescent="0.3">
+    <row r="31" spans="8:35" x14ac:dyDescent="0.3">
       <c r="I31">
         <f>36093 - 30183</f>
         <v>5910</v>
@@ -5464,7 +5567,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="32" spans="9:35" x14ac:dyDescent="0.3">
+    <row r="32" spans="8:35" x14ac:dyDescent="0.3">
       <c r="I32">
         <f>613581-452745</f>
         <v>160836</v>
@@ -5488,7 +5591,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="33" spans="9:35" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="33" spans="7:35" ht="28.8" x14ac:dyDescent="0.3">
       <c r="I33">
         <f>I32/I31</f>
         <v>27.214213197969542</v>
@@ -5566,7 +5669,7 @@
         <v>Master's Gross</v>
       </c>
     </row>
-    <row r="34" spans="9:35" x14ac:dyDescent="0.3">
+    <row r="34" spans="7:35" x14ac:dyDescent="0.3">
       <c r="L34">
         <v>14</v>
       </c>
@@ -5583,7 +5686,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="35" spans="9:35" x14ac:dyDescent="0.3">
+    <row r="35" spans="7:35" x14ac:dyDescent="0.3">
       <c r="L35">
         <v>15</v>
       </c>
@@ -5600,7 +5703,16 @@
         <v>15</v>
       </c>
     </row>
-    <row r="36" spans="9:35" x14ac:dyDescent="0.3">
+    <row r="36" spans="7:35" x14ac:dyDescent="0.3">
+      <c r="H36">
+        <v>57539</v>
+      </c>
+      <c r="I36">
+        <v>26046.306710515335</v>
+      </c>
+      <c r="J36">
+        <v>31492.693289484665</v>
+      </c>
       <c r="L36">
         <v>16</v>
       </c>
@@ -5627,7 +5739,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="37" spans="9:35" x14ac:dyDescent="0.3">
+    <row r="37" spans="7:35" x14ac:dyDescent="0.3">
       <c r="L37">
         <v>17</v>
       </c>
@@ -5651,7 +5763,14 @@
         <v>17</v>
       </c>
     </row>
-    <row r="38" spans="9:35" x14ac:dyDescent="0.3">
+    <row r="38" spans="7:35" x14ac:dyDescent="0.3">
+      <c r="G38">
+        <f>22*57539</f>
+        <v>1265858</v>
+      </c>
+      <c r="H38" s="8" t="s">
+        <v>42</v>
+      </c>
       <c r="L38">
         <v>18</v>
       </c>
@@ -5660,7 +5779,7 @@
       </c>
       <c r="N38" s="7"/>
       <c r="O38" s="7">
-        <f t="shared" ref="O38:O58" si="8">O37+M38</f>
+        <f t="shared" ref="O38:O58" si="13">O37+M38</f>
         <v>125286</v>
       </c>
       <c r="Q38">
@@ -5707,7 +5826,14 @@
       </c>
       <c r="AI38" s="7"/>
     </row>
-    <row r="39" spans="9:35" x14ac:dyDescent="0.3">
+    <row r="39" spans="7:35" x14ac:dyDescent="0.3">
+      <c r="G39">
+        <f>31492.69 - G38</f>
+        <v>-1234365.31</v>
+      </c>
+      <c r="H39" t="s">
+        <v>43</v>
+      </c>
       <c r="L39">
         <v>19</v>
       </c>
@@ -5715,7 +5841,7 @@
         <v>41762</v>
       </c>
       <c r="O39" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>167048</v>
       </c>
       <c r="Q39">
@@ -5759,7 +5885,7 @@
       </c>
       <c r="AI39" s="7"/>
     </row>
-    <row r="40" spans="9:35" x14ac:dyDescent="0.3">
+    <row r="40" spans="7:35" x14ac:dyDescent="0.3">
       <c r="L40">
         <v>20</v>
       </c>
@@ -5767,7 +5893,7 @@
         <v>41762</v>
       </c>
       <c r="O40" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>208810</v>
       </c>
       <c r="Q40">
@@ -5777,7 +5903,7 @@
         <v>39250</v>
       </c>
       <c r="T40" s="7">
-        <f t="shared" ref="T40:T58" si="9">T39+R40</f>
+        <f t="shared" ref="T40:T58" si="14">T39+R40</f>
         <v>117750</v>
       </c>
       <c r="V40">
@@ -5788,11 +5914,11 @@
       </c>
       <c r="X40" s="6">
         <f>$I$4/2</f>
-        <v>13023.153355257667</v>
+        <v>16670.124662980634</v>
       </c>
       <c r="Y40" s="7">
         <f>W40-X40</f>
-        <v>34234.846644742334</v>
+        <v>30587.875337019366</v>
       </c>
       <c r="AA40">
         <v>20</v>
@@ -5815,7 +5941,7 @@
       </c>
       <c r="AI40" s="7"/>
     </row>
-    <row r="41" spans="9:35" x14ac:dyDescent="0.3">
+    <row r="41" spans="7:35" x14ac:dyDescent="0.3">
       <c r="L41">
         <v>21</v>
       </c>
@@ -5823,7 +5949,7 @@
         <v>41762</v>
       </c>
       <c r="O41" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>250572</v>
       </c>
       <c r="Q41">
@@ -5833,7 +5959,7 @@
         <v>39250</v>
       </c>
       <c r="T41" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>157000</v>
       </c>
       <c r="V41">
@@ -5844,11 +5970,11 @@
       </c>
       <c r="X41" s="6">
         <f>X40-(($H$4*12)/2)</f>
-        <v>11720.8380197319</v>
+        <v>15003.11219668257</v>
       </c>
       <c r="Y41" s="7">
         <f>W41+Y40</f>
-        <v>81492.846644742327</v>
+        <v>77845.875337019359</v>
       </c>
       <c r="AA41">
         <v>21</v>
@@ -5871,7 +5997,7 @@
       </c>
       <c r="AI41" s="7"/>
     </row>
-    <row r="42" spans="9:35" x14ac:dyDescent="0.3">
+    <row r="42" spans="7:35" x14ac:dyDescent="0.3">
       <c r="L42">
         <v>22</v>
       </c>
@@ -5880,7 +6006,7 @@
       </c>
       <c r="N42" s="6"/>
       <c r="O42" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>292334</v>
       </c>
       <c r="Q42">
@@ -5890,7 +6016,7 @@
         <v>39250</v>
       </c>
       <c r="T42" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>196250</v>
       </c>
       <c r="V42">
@@ -5900,12 +6026,12 @@
         <v>47258</v>
       </c>
       <c r="X42" s="6">
-        <f t="shared" ref="X42:X50" si="10">X41-(($H$4*12)/2)</f>
-        <v>10418.522684206133</v>
+        <f t="shared" ref="X42:X50" si="15">X41-(($H$4*12)/2)</f>
+        <v>13336.099730384507</v>
       </c>
       <c r="Y42" s="7">
         <f>W42+Y41</f>
-        <v>128750.84664474233</v>
+        <v>125103.87533701936</v>
       </c>
       <c r="AA42">
         <v>22</v>
@@ -5915,11 +6041,11 @@
       </c>
       <c r="AC42" s="6">
         <f>$I$4</f>
-        <v>26046.306710515335</v>
+        <v>33340.249325961267</v>
       </c>
       <c r="AD42" s="7">
         <f>AB42-AC42</f>
-        <v>30783.693289484665</v>
+        <v>23489.750674038733</v>
       </c>
       <c r="AF42">
         <v>22</v>
@@ -5932,7 +6058,7 @@
       </c>
       <c r="AI42" s="7"/>
     </row>
-    <row r="43" spans="9:35" x14ac:dyDescent="0.3">
+    <row r="43" spans="7:35" x14ac:dyDescent="0.3">
       <c r="L43">
         <v>23</v>
       </c>
@@ -5941,7 +6067,7 @@
       </c>
       <c r="N43" s="6"/>
       <c r="O43" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>334096</v>
       </c>
       <c r="Q43">
@@ -5951,7 +6077,7 @@
         <v>39250</v>
       </c>
       <c r="T43" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>235500</v>
       </c>
       <c r="V43">
@@ -5961,12 +6087,12 @@
         <v>47258</v>
       </c>
       <c r="X43" s="6">
-        <f t="shared" si="10"/>
-        <v>9116.2073486803656</v>
+        <f t="shared" si="15"/>
+        <v>11669.087264086444</v>
       </c>
       <c r="Y43" s="7">
-        <f t="shared" ref="Y43:Y58" si="11">W43+Y42</f>
-        <v>176008.84664474233</v>
+        <f t="shared" ref="Y43:Y58" si="16">W43+Y42</f>
+        <v>172361.87533701936</v>
       </c>
       <c r="AA43">
         <v>23</v>
@@ -5976,11 +6102,11 @@
       </c>
       <c r="AC43" s="6">
         <f>AC42-($H$4*12)</f>
-        <v>23441.6760394638</v>
+        <v>30006.224393365141</v>
       </c>
       <c r="AD43" s="7">
         <f>AB43+AD42</f>
-        <v>87613.693289484669</v>
+        <v>80319.750674038733</v>
       </c>
       <c r="AF43">
         <v>23</v>
@@ -5993,7 +6119,7 @@
       </c>
       <c r="AI43" s="7"/>
     </row>
-    <row r="44" spans="9:35" x14ac:dyDescent="0.3">
+    <row r="44" spans="7:35" x14ac:dyDescent="0.3">
       <c r="L44">
         <v>24</v>
       </c>
@@ -6002,7 +6128,7 @@
       </c>
       <c r="N44" s="6"/>
       <c r="O44" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>375858</v>
       </c>
       <c r="Q44">
@@ -6012,7 +6138,7 @@
         <v>39250</v>
       </c>
       <c r="T44" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>274750</v>
       </c>
       <c r="V44">
@@ -6022,12 +6148,12 @@
         <v>47258</v>
       </c>
       <c r="X44" s="6">
-        <f t="shared" si="10"/>
-        <v>7813.8920131545992</v>
+        <f t="shared" si="15"/>
+        <v>10002.07479778838</v>
       </c>
       <c r="Y44" s="7">
-        <f t="shared" si="11"/>
-        <v>223266.84664474233</v>
+        <f t="shared" si="16"/>
+        <v>219619.87533701936</v>
       </c>
       <c r="AA44">
         <v>24</v>
@@ -6036,12 +6162,12 @@
         <v>56830</v>
       </c>
       <c r="AC44" s="6">
-        <f t="shared" ref="AC44:AC52" si="12">AC43-($H$4*12)</f>
-        <v>20837.045368412266</v>
+        <f t="shared" ref="AC44:AC52" si="17">AC43-($H$4*12)</f>
+        <v>26672.199460769014</v>
       </c>
       <c r="AD44" s="7">
         <f>AB44+AD43</f>
-        <v>144443.69328948465</v>
+        <v>137149.75067403872</v>
       </c>
       <c r="AF44">
         <v>24</v>
@@ -6058,7 +6184,7 @@
         <v>72837</v>
       </c>
     </row>
-    <row r="45" spans="9:35" x14ac:dyDescent="0.3">
+    <row r="45" spans="7:35" x14ac:dyDescent="0.3">
       <c r="L45">
         <v>25</v>
       </c>
@@ -6067,7 +6193,7 @@
       </c>
       <c r="N45" s="6"/>
       <c r="O45" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>417620</v>
       </c>
       <c r="Q45">
@@ -6077,7 +6203,7 @@
         <v>39250</v>
       </c>
       <c r="T45" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>314000</v>
       </c>
       <c r="V45">
@@ -6087,12 +6213,12 @@
         <v>47258</v>
       </c>
       <c r="X45" s="6">
-        <f t="shared" si="10"/>
-        <v>6511.5766776288328</v>
+        <f t="shared" si="15"/>
+        <v>8335.0623314903169</v>
       </c>
       <c r="Y45" s="7">
-        <f t="shared" si="11"/>
-        <v>270524.8466447423</v>
+        <f t="shared" si="16"/>
+        <v>266877.87533701933</v>
       </c>
       <c r="AA45">
         <v>25</v>
@@ -6101,12 +6227,12 @@
         <v>56830</v>
       </c>
       <c r="AC45" s="6">
-        <f t="shared" si="12"/>
-        <v>18232.414697360731</v>
+        <f t="shared" si="17"/>
+        <v>23338.174528172887</v>
       </c>
       <c r="AD45" s="7">
-        <f t="shared" ref="AD45:AD58" si="13">AB45+AD44</f>
-        <v>201273.69328948465</v>
+        <f t="shared" ref="AD45:AD58" si="18">AB45+AD44</f>
+        <v>193979.75067403872</v>
       </c>
       <c r="AF45">
         <v>25</v>
@@ -6116,14 +6242,14 @@
       </c>
       <c r="AH45" s="6">
         <f>AH44-($H$4*12*1.5)</f>
-        <v>-3906.9460065773001</v>
+        <v>-5001.0373988941901</v>
       </c>
       <c r="AI45" s="7">
-        <f t="shared" ref="AI45:AI58" si="14">AG45+AI44</f>
+        <f t="shared" ref="AI45:AI58" si="19">AG45+AI44</f>
         <v>145674</v>
       </c>
     </row>
-    <row r="46" spans="9:35" x14ac:dyDescent="0.3">
+    <row r="46" spans="7:35" x14ac:dyDescent="0.3">
       <c r="L46">
         <v>26</v>
       </c>
@@ -6132,7 +6258,7 @@
       </c>
       <c r="N46" s="6"/>
       <c r="O46" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>459382</v>
       </c>
       <c r="Q46">
@@ -6142,7 +6268,7 @@
         <v>39250</v>
       </c>
       <c r="T46" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>353250</v>
       </c>
       <c r="V46">
@@ -6152,12 +6278,12 @@
         <v>47258</v>
       </c>
       <c r="X46" s="6">
-        <f t="shared" si="10"/>
-        <v>5209.2613421030665</v>
+        <f t="shared" si="15"/>
+        <v>6668.0498651922535</v>
       </c>
       <c r="Y46" s="7">
-        <f t="shared" si="11"/>
-        <v>317782.8466447423</v>
+        <f t="shared" si="16"/>
+        <v>314135.87533701933</v>
       </c>
       <c r="AA46">
         <v>26</v>
@@ -6166,12 +6292,12 @@
         <v>56830</v>
       </c>
       <c r="AC46" s="6">
-        <f t="shared" si="12"/>
-        <v>15627.784026309198</v>
+        <f t="shared" si="17"/>
+        <v>20004.14959557676</v>
       </c>
       <c r="AD46" s="7">
-        <f t="shared" si="13"/>
-        <v>258103.69328948465</v>
+        <f t="shared" si="18"/>
+        <v>250809.75067403872</v>
       </c>
       <c r="AF46">
         <v>26</v>
@@ -6180,15 +6306,15 @@
         <v>72837</v>
       </c>
       <c r="AH46" s="6">
-        <f t="shared" ref="AH46:AH54" si="15">AH45-($H$4*12*1.5)</f>
-        <v>-7813.8920131546001</v>
+        <f t="shared" ref="AH46:AH54" si="20">AH45-($H$4*12*1.5)</f>
+        <v>-10002.07479778838</v>
       </c>
       <c r="AI46" s="7">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>218511</v>
       </c>
     </row>
-    <row r="47" spans="9:35" x14ac:dyDescent="0.3">
+    <row r="47" spans="7:35" x14ac:dyDescent="0.3">
       <c r="L47">
         <v>27</v>
       </c>
@@ -6197,7 +6323,7 @@
       </c>
       <c r="N47" s="6"/>
       <c r="O47" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>501144</v>
       </c>
       <c r="Q47">
@@ -6207,7 +6333,7 @@
         <v>39250</v>
       </c>
       <c r="T47" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>392500</v>
       </c>
       <c r="V47">
@@ -6217,12 +6343,12 @@
         <v>47258</v>
       </c>
       <c r="X47" s="6">
-        <f t="shared" si="10"/>
-        <v>3906.9460065773001</v>
+        <f t="shared" si="15"/>
+        <v>5001.0373988941901</v>
       </c>
       <c r="Y47" s="7">
-        <f t="shared" si="11"/>
-        <v>365040.8466447423</v>
+        <f t="shared" si="16"/>
+        <v>361393.87533701933</v>
       </c>
       <c r="AA47">
         <v>27</v>
@@ -6231,12 +6357,12 @@
         <v>56830</v>
       </c>
       <c r="AC47" s="6">
-        <f t="shared" si="12"/>
-        <v>13023.153355257666</v>
+        <f t="shared" si="17"/>
+        <v>16670.124662980634</v>
       </c>
       <c r="AD47" s="7">
-        <f t="shared" si="13"/>
-        <v>314933.69328948465</v>
+        <f t="shared" si="18"/>
+        <v>307639.75067403872</v>
       </c>
       <c r="AF47">
         <v>27</v>
@@ -6245,15 +6371,15 @@
         <v>72837</v>
       </c>
       <c r="AH47" s="6">
-        <f t="shared" si="15"/>
-        <v>-11720.8380197319</v>
+        <f t="shared" si="20"/>
+        <v>-15003.11219668257</v>
       </c>
       <c r="AI47" s="7">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>291348</v>
       </c>
     </row>
-    <row r="48" spans="9:35" x14ac:dyDescent="0.3">
+    <row r="48" spans="7:35" x14ac:dyDescent="0.3">
       <c r="L48">
         <v>28</v>
       </c>
@@ -6262,7 +6388,7 @@
       </c>
       <c r="N48" s="6"/>
       <c r="O48" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>542906</v>
       </c>
       <c r="Q48">
@@ -6272,7 +6398,7 @@
         <v>39250</v>
       </c>
       <c r="T48" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>431750</v>
       </c>
       <c r="V48">
@@ -6282,12 +6408,12 @@
         <v>47258</v>
       </c>
       <c r="X48" s="6">
-        <f t="shared" si="10"/>
-        <v>2604.6306710515337</v>
+        <f t="shared" si="15"/>
+        <v>3334.0249325961267</v>
       </c>
       <c r="Y48" s="7">
-        <f t="shared" si="11"/>
-        <v>412298.8466447423</v>
+        <f t="shared" si="16"/>
+        <v>408651.87533701933</v>
       </c>
       <c r="AA48">
         <v>28</v>
@@ -6296,12 +6422,12 @@
         <v>56830</v>
       </c>
       <c r="AC48" s="6">
-        <f t="shared" si="12"/>
-        <v>10418.522684206133</v>
+        <f t="shared" si="17"/>
+        <v>13336.099730384507</v>
       </c>
       <c r="AD48" s="7">
-        <f t="shared" si="13"/>
-        <v>371763.69328948465</v>
+        <f t="shared" si="18"/>
+        <v>364469.75067403872</v>
       </c>
       <c r="AF48">
         <v>28</v>
@@ -6310,11 +6436,11 @@
         <v>72837</v>
       </c>
       <c r="AH48" s="6">
-        <f t="shared" si="15"/>
-        <v>-15627.7840263092</v>
+        <f t="shared" si="20"/>
+        <v>-20004.14959557676</v>
       </c>
       <c r="AI48" s="7">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>364185</v>
       </c>
     </row>
@@ -6327,7 +6453,7 @@
       </c>
       <c r="N49" s="6"/>
       <c r="O49" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>584668</v>
       </c>
       <c r="Q49">
@@ -6337,7 +6463,7 @@
         <v>39250</v>
       </c>
       <c r="T49" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>471000</v>
       </c>
       <c r="V49">
@@ -6347,12 +6473,12 @@
         <v>47258</v>
       </c>
       <c r="X49" s="6">
-        <f t="shared" si="10"/>
-        <v>1302.3153355257671</v>
+        <f t="shared" si="15"/>
+        <v>1667.0124662980634</v>
       </c>
       <c r="Y49" s="7">
-        <f t="shared" si="11"/>
-        <v>459556.8466447423</v>
+        <f t="shared" si="16"/>
+        <v>455909.87533701933</v>
       </c>
       <c r="AA49">
         <v>29</v>
@@ -6361,12 +6487,12 @@
         <v>56830</v>
       </c>
       <c r="AC49" s="6">
-        <f t="shared" si="12"/>
-        <v>7813.8920131546001</v>
+        <f t="shared" si="17"/>
+        <v>10002.07479778838</v>
       </c>
       <c r="AD49" s="7">
-        <f t="shared" si="13"/>
-        <v>428593.69328948465</v>
+        <f t="shared" si="18"/>
+        <v>421299.75067403872</v>
       </c>
       <c r="AF49">
         <v>29</v>
@@ -6375,11 +6501,11 @@
         <v>72837</v>
       </c>
       <c r="AH49" s="6">
-        <f t="shared" si="15"/>
-        <v>-19534.730032886502</v>
+        <f t="shared" si="20"/>
+        <v>-25005.186994470951</v>
       </c>
       <c r="AI49" s="7">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>437022</v>
       </c>
     </row>
@@ -6392,7 +6518,7 @@
       </c>
       <c r="N50" s="6"/>
       <c r="O50" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>626430</v>
       </c>
       <c r="Q50">
@@ -6402,7 +6528,7 @@
         <v>39250</v>
       </c>
       <c r="T50" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>510250</v>
       </c>
       <c r="V50">
@@ -6412,12 +6538,12 @@
         <v>47258</v>
       </c>
       <c r="X50" s="6">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="Y50" s="7">
-        <f t="shared" si="11"/>
-        <v>506814.8466447423</v>
+        <f t="shared" si="16"/>
+        <v>503167.87533701933</v>
       </c>
       <c r="AA50">
         <v>30</v>
@@ -6426,12 +6552,12 @@
         <v>56830</v>
       </c>
       <c r="AC50" s="6">
-        <f t="shared" si="12"/>
-        <v>5209.2613421030674</v>
+        <f t="shared" si="17"/>
+        <v>6668.0498651922535</v>
       </c>
       <c r="AD50" s="7">
-        <f t="shared" si="13"/>
-        <v>485423.69328948465</v>
+        <f t="shared" si="18"/>
+        <v>478129.75067403872</v>
       </c>
       <c r="AF50">
         <v>30</v>
@@ -6440,11 +6566,11 @@
         <v>72837</v>
       </c>
       <c r="AH50" s="6">
-        <f t="shared" si="15"/>
-        <v>-23441.676039463804</v>
+        <f t="shared" si="20"/>
+        <v>-30006.224393365141</v>
       </c>
       <c r="AI50" s="7">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>509859</v>
       </c>
     </row>
@@ -6457,7 +6583,7 @@
       </c>
       <c r="N51" s="6"/>
       <c r="O51" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>668192</v>
       </c>
       <c r="Q51">
@@ -6467,7 +6593,7 @@
         <v>39250</v>
       </c>
       <c r="T51" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>549500</v>
       </c>
       <c r="V51">
@@ -6478,8 +6604,8 @@
       </c>
       <c r="X51" s="6"/>
       <c r="Y51" s="7">
-        <f t="shared" si="11"/>
-        <v>554072.8466447423</v>
+        <f t="shared" si="16"/>
+        <v>550425.87533701933</v>
       </c>
       <c r="AA51">
         <v>31</v>
@@ -6488,12 +6614,12 @@
         <v>56830</v>
       </c>
       <c r="AC51" s="6">
-        <f t="shared" si="12"/>
-        <v>2604.6306710515341</v>
+        <f t="shared" si="17"/>
+        <v>3334.0249325961267</v>
       </c>
       <c r="AD51" s="7">
-        <f t="shared" si="13"/>
-        <v>542253.6932894846</v>
+        <f t="shared" si="18"/>
+        <v>534959.75067403866</v>
       </c>
       <c r="AF51">
         <v>31</v>
@@ -6502,11 +6628,11 @@
         <v>72837</v>
       </c>
       <c r="AH51" s="6">
-        <f t="shared" si="15"/>
-        <v>-27348.622046041106</v>
+        <f t="shared" si="20"/>
+        <v>-35007.261792259334</v>
       </c>
       <c r="AI51" s="7">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>582696</v>
       </c>
     </row>
@@ -6519,7 +6645,7 @@
       </c>
       <c r="N52" s="6"/>
       <c r="O52" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>709954</v>
       </c>
       <c r="Q52">
@@ -6529,7 +6655,7 @@
         <v>39250</v>
       </c>
       <c r="T52" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>588750</v>
       </c>
       <c r="V52">
@@ -6540,8 +6666,8 @@
       </c>
       <c r="X52" s="6"/>
       <c r="Y52" s="7">
-        <f t="shared" si="11"/>
-        <v>601330.8466447423</v>
+        <f t="shared" si="16"/>
+        <v>597683.87533701933</v>
       </c>
       <c r="AA52">
         <v>32</v>
@@ -6550,12 +6676,12 @@
         <v>56830</v>
       </c>
       <c r="AC52" s="6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="AD52" s="7">
-        <f t="shared" si="13"/>
-        <v>599083.6932894846</v>
+        <f t="shared" si="18"/>
+        <v>591789.75067403866</v>
       </c>
       <c r="AF52">
         <v>32</v>
@@ -6564,11 +6690,11 @@
         <v>72837</v>
       </c>
       <c r="AH52" s="6">
-        <f t="shared" si="15"/>
-        <v>-31255.568052618408</v>
+        <f t="shared" si="20"/>
+        <v>-40008.299191153521</v>
       </c>
       <c r="AI52" s="7">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>655533</v>
       </c>
     </row>
@@ -6581,7 +6707,7 @@
       </c>
       <c r="N53" s="6"/>
       <c r="O53" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>751716</v>
       </c>
       <c r="Q53">
@@ -6591,7 +6717,7 @@
         <v>39250</v>
       </c>
       <c r="T53" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>628000</v>
       </c>
       <c r="V53">
@@ -6602,8 +6728,8 @@
       </c>
       <c r="X53" s="6"/>
       <c r="Y53" s="7">
-        <f t="shared" si="11"/>
-        <v>648588.8466447423</v>
+        <f t="shared" si="16"/>
+        <v>644941.87533701933</v>
       </c>
       <c r="AA53">
         <v>33</v>
@@ -6613,8 +6739,8 @@
       </c>
       <c r="AC53" s="6"/>
       <c r="AD53" s="7">
-        <f t="shared" si="13"/>
-        <v>655913.6932894846</v>
+        <f t="shared" si="18"/>
+        <v>648619.75067403866</v>
       </c>
       <c r="AF53">
         <v>33</v>
@@ -6623,11 +6749,11 @@
         <v>72837</v>
       </c>
       <c r="AH53" s="6">
-        <f t="shared" si="15"/>
-        <v>-35162.51405919571</v>
+        <f t="shared" si="20"/>
+        <v>-45009.336590047707</v>
       </c>
       <c r="AI53" s="7">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>728370</v>
       </c>
     </row>
@@ -6640,7 +6766,7 @@
       </c>
       <c r="N54" s="6"/>
       <c r="O54" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>793478</v>
       </c>
       <c r="Q54">
@@ -6650,7 +6776,7 @@
         <v>39250</v>
       </c>
       <c r="T54" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>667250</v>
       </c>
       <c r="V54">
@@ -6661,8 +6787,8 @@
       </c>
       <c r="X54" s="6"/>
       <c r="Y54" s="7">
-        <f t="shared" si="11"/>
-        <v>695846.8466447423</v>
+        <f t="shared" si="16"/>
+        <v>692199.87533701933</v>
       </c>
       <c r="AA54">
         <v>34</v>
@@ -6672,8 +6798,8 @@
       </c>
       <c r="AC54" s="6"/>
       <c r="AD54" s="7">
-        <f t="shared" si="13"/>
-        <v>712743.6932894846</v>
+        <f t="shared" si="18"/>
+        <v>705449.75067403866</v>
       </c>
       <c r="AF54">
         <v>34</v>
@@ -6682,11 +6808,11 @@
         <v>72837</v>
       </c>
       <c r="AH54" s="6">
-        <f t="shared" si="15"/>
-        <v>-39069.460065773012</v>
+        <f t="shared" si="20"/>
+        <v>-50010.373988941894</v>
       </c>
       <c r="AI54" s="7">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>801207</v>
       </c>
     </row>
@@ -6698,7 +6824,7 @@
         <v>41762</v>
       </c>
       <c r="O55" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>835240</v>
       </c>
       <c r="Q55">
@@ -6708,7 +6834,7 @@
         <v>39250</v>
       </c>
       <c r="T55" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>706500</v>
       </c>
       <c r="V55">
@@ -6718,8 +6844,8 @@
         <v>47258</v>
       </c>
       <c r="Y55" s="7">
-        <f t="shared" si="11"/>
-        <v>743104.8466447423</v>
+        <f t="shared" si="16"/>
+        <v>739457.87533701933</v>
       </c>
       <c r="AA55">
         <v>35</v>
@@ -6728,8 +6854,8 @@
         <v>56830</v>
       </c>
       <c r="AD55" s="7">
-        <f t="shared" si="13"/>
-        <v>769573.6932894846</v>
+        <f t="shared" si="18"/>
+        <v>762279.75067403866</v>
       </c>
       <c r="AF55">
         <v>35</v>
@@ -6738,7 +6864,7 @@
         <v>72837</v>
       </c>
       <c r="AI55" s="7">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>874044</v>
       </c>
     </row>
@@ -6750,7 +6876,7 @@
         <v>41762</v>
       </c>
       <c r="O56" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>877002</v>
       </c>
       <c r="Q56">
@@ -6760,7 +6886,7 @@
         <v>39250</v>
       </c>
       <c r="T56" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>745750</v>
       </c>
       <c r="V56">
@@ -6770,8 +6896,8 @@
         <v>47258</v>
       </c>
       <c r="Y56" s="7">
-        <f t="shared" si="11"/>
-        <v>790362.8466447423</v>
+        <f t="shared" si="16"/>
+        <v>786715.87533701933</v>
       </c>
       <c r="AA56">
         <v>36</v>
@@ -6780,8 +6906,8 @@
         <v>56830</v>
       </c>
       <c r="AD56" s="7">
-        <f t="shared" si="13"/>
-        <v>826403.6932894846</v>
+        <f t="shared" si="18"/>
+        <v>819109.75067403866</v>
       </c>
       <c r="AF56">
         <v>36</v>
@@ -6790,7 +6916,7 @@
         <v>72837</v>
       </c>
       <c r="AI56" s="7">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>946881</v>
       </c>
     </row>
@@ -6802,7 +6928,7 @@
         <v>41762</v>
       </c>
       <c r="O57" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>918764</v>
       </c>
       <c r="Q57">
@@ -6812,7 +6938,7 @@
         <v>39250</v>
       </c>
       <c r="T57" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>785000</v>
       </c>
       <c r="V57">
@@ -6822,8 +6948,8 @@
         <v>47258</v>
       </c>
       <c r="Y57" s="7">
-        <f t="shared" si="11"/>
-        <v>837620.8466447423</v>
+        <f t="shared" si="16"/>
+        <v>833973.87533701933</v>
       </c>
       <c r="AA57">
         <v>37</v>
@@ -6832,8 +6958,8 @@
         <v>56830</v>
       </c>
       <c r="AD57" s="7">
-        <f t="shared" si="13"/>
-        <v>883233.6932894846</v>
+        <f t="shared" si="18"/>
+        <v>875939.75067403866</v>
       </c>
       <c r="AF57">
         <v>37</v>
@@ -6842,7 +6968,7 @@
         <v>72837</v>
       </c>
       <c r="AI57" s="7">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>1019718</v>
       </c>
     </row>
@@ -6854,7 +6980,7 @@
         <v>41762</v>
       </c>
       <c r="O58" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>960526</v>
       </c>
       <c r="Q58">
@@ -6864,7 +6990,7 @@
         <v>39250</v>
       </c>
       <c r="T58" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>824250</v>
       </c>
       <c r="V58">
@@ -6874,8 +7000,8 @@
         <v>47258</v>
       </c>
       <c r="Y58" s="7">
-        <f t="shared" si="11"/>
-        <v>884878.8466447423</v>
+        <f t="shared" si="16"/>
+        <v>881231.87533701933</v>
       </c>
       <c r="AA58">
         <v>38</v>
@@ -6884,8 +7010,8 @@
         <v>56830</v>
       </c>
       <c r="AD58" s="7">
-        <f t="shared" si="13"/>
-        <v>940063.6932894846</v>
+        <f t="shared" si="18"/>
+        <v>932769.75067403866</v>
       </c>
       <c r="AF58">
         <v>38</v>
@@ -6894,7 +7020,7 @@
         <v>72837</v>
       </c>
       <c r="AI58" s="7">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>1092555</v>
       </c>
     </row>
@@ -6903,15 +7029,15 @@
         <v>41763</v>
       </c>
       <c r="O59" s="7">
-        <f t="shared" ref="O59:O60" si="16">O58+M59</f>
+        <f t="shared" ref="O59:O60" si="21">O58+M59</f>
         <v>1002289</v>
       </c>
       <c r="AB59">
         <v>56831</v>
       </c>
       <c r="AD59" s="7">
-        <f t="shared" ref="AD59" si="17">AB59+AD58</f>
-        <v>996894.6932894846</v>
+        <f t="shared" ref="AD59" si="22">AB59+AD58</f>
+        <v>989600.75067403866</v>
       </c>
     </row>
     <row r="60" spans="12:35" x14ac:dyDescent="0.3">
@@ -6919,15 +7045,15 @@
         <v>41764</v>
       </c>
       <c r="O60" s="7">
-        <f t="shared" si="16"/>
+        <f t="shared" si="21"/>
         <v>1044053</v>
       </c>
       <c r="AB60">
         <v>56832</v>
       </c>
       <c r="AD60" s="7">
-        <f t="shared" ref="AD60" si="18">AB60+AD59</f>
-        <v>1053726.6932894846</v>
+        <f t="shared" ref="AD60" si="23">AB60+AD59</f>
+        <v>1046432.7506740387</v>
       </c>
     </row>
   </sheetData>

</xml_diff>